<commit_message>
Added reading 'isGecorreleerd' from acceptance test files. ASK-87
</commit_message>
<xml_diff>
--- a/test/Assembly.Kernel.Acceptance.TestUtil/test-data/Benchmarktool assemblage - Failure mechanism with length-effect.xlsx
+++ b/test/Assembly.Kernel.Acceptance.TestUtil/test-data/Benchmarktool assemblage - Failure mechanism with length-effect.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3F4172-C461-473A-AE45-2FBCBC81C2DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1FBC67-EF03-40B3-926A-900891FCE256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="68">
   <si>
     <t>Faalpad</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Pfalen tussenresultaten</t>
+  </si>
+  <si>
+    <t>Gecorreleerd</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Z37"/>
+  <dimension ref="B2:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N7" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,15 +958,15 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6">
-        <v>6.0666886439917911E-2</v>
+        <v>67</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6">
         <v>6.0666886439917911E-2</v>
@@ -971,347 +974,283 @@
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C8" s="6">
-        <f>IFERROR(MAX(Y15:Y34),"GR")</f>
-        <v>3.3120289000265313E-2</v>
+        <v>6.0666886439917911E-2</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="6">
-        <f>MAX(Z15:Z34)</f>
+        <f>IFERROR(MAX(Y16:Y35),"GR")</f>
         <v>3.3120289000265313E-2</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="6">
+        <f>MAX(Z16:Z35)</f>
+        <v>3.3120289000265313E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="6">
-        <f>IFERROR(1-PRODUCT(Q15:Q34),"GR")</f>
+      <c r="C11" s="6">
+        <f>IFERROR(1-PRODUCT(Q16:Q35),"GR")</f>
         <v>6.0666875893912287E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="33">
-        <f>1-PRODUCT(R15:R34)</f>
+      <c r="C12" s="33">
+        <f>1-PRODUCT(R16:R35)</f>
         <v>6.0666875893912287E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
-      <c r="C12" s="24"/>
-    </row>
-    <row r="14" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q14" t="s">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B13" s="38"/>
+      <c r="C13" s="24"/>
+    </row>
+    <row r="15" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:26" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
+    <row r="16" spans="2:26" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="O16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="2" t="s">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="R16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="S16" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="T15" s="12" t="s">
+      <c r="T16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="U15" s="13" t="s">
+      <c r="U16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="V15" s="13" t="s">
+      <c r="V16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="W15" s="14"/>
-      <c r="X15" s="13" t="s">
+      <c r="W16" s="14"/>
+      <c r="X16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Y15" s="12" t="s">
+      <c r="Y16" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="39" t="s">
+      <c r="Z16" s="39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C17" s="14">
         <v>0</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D17" s="14">
         <v>0.16564654600000001</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E17" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F17" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G17" s="17">
         <v>2.6412322020898397E-4</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H17" s="18">
         <v>3.224580190703381E-4</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="19">
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19">
         <v>2.6412322020898397E-4</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M17" s="17">
         <v>3.224580190703381E-4</v>
       </c>
-      <c r="N16" s="20">
+      <c r="N17" s="20">
         <v>1.2208620613333334</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="O17" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q17" s="22">
         <v>0.99967754198092962</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R17" s="23">
         <v>0.99967754198092962</v>
       </c>
-      <c r="S16" s="23">
+      <c r="S17" s="23">
         <v>7.6331610640396367E-3</v>
       </c>
-      <c r="T16" s="23">
+      <c r="T17" s="23">
         <v>7.6331610640396367E-3</v>
       </c>
-      <c r="U16" s="24">
+      <c r="U17" s="24">
         <v>3.3333333333333332E-4</v>
       </c>
-      <c r="V16" s="24">
+      <c r="V17" s="24">
         <v>4</v>
       </c>
-      <c r="W16" s="24" t="s">
+      <c r="W17" s="24" t="s">
         <v>52</v>
-      </c>
-      <c r="X16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="23">
-        <f>1-Q16</f>
-        <v>3.2245801907038185E-4</v>
-      </c>
-      <c r="Z16" s="6">
-        <f>1-R16</f>
-        <v>3.2245801907038185E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="24">
-        <v>0.16564654600000001</v>
-      </c>
-      <c r="D17" s="24">
-        <v>0.342187662</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="23">
-        <v>2.6809621636045101E-2</v>
-      </c>
-      <c r="K17" s="6">
-        <v>3.3120289000265299E-2</v>
-      </c>
-      <c r="L17" s="22">
-        <v>2.6809621636045101E-2</v>
-      </c>
-      <c r="M17" s="23">
-        <v>3.3120289000265299E-2</v>
-      </c>
-      <c r="N17" s="27">
-        <v>1.2353881546666667</v>
-      </c>
-      <c r="O17" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q17" s="22">
-        <v>0.96687971099973469</v>
-      </c>
-      <c r="R17" s="23">
-        <v>0.96687971099973469</v>
-      </c>
-      <c r="S17" s="23">
-        <v>0.77479806528170336</v>
-      </c>
-      <c r="T17" s="23">
-        <v>0.77479806528170336</v>
-      </c>
-      <c r="U17" s="24">
-        <v>1</v>
-      </c>
-      <c r="V17" s="24">
-        <v>7</v>
-      </c>
-      <c r="W17" s="24" t="s">
-        <v>53</v>
       </c>
       <c r="X17" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y17" s="23">
-        <f t="shared" ref="Y17:Z35" si="0">1-Q17</f>
-        <v>3.3120289000265313E-2</v>
+        <f>1-Q17</f>
+        <v>3.2245801907038185E-4</v>
       </c>
       <c r="Z17" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3120289000265313E-2</v>
+        <f>1-R17</f>
+        <v>3.2245801907038185E-4</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="24">
+        <v>0.16564654600000001</v>
+      </c>
+      <c r="D18" s="24">
         <v>0.342187662</v>
-      </c>
-      <c r="D18" s="24">
-        <v>0.995927067</v>
       </c>
       <c r="E18" s="26" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="23">
-        <v>5.62288806246054E-10</v>
-      </c>
-      <c r="H18" s="6">
-        <v>1.0524092724239948E-9</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="J18" s="23">
+        <v>2.6809621636045101E-2</v>
+      </c>
+      <c r="K18" s="6">
+        <v>3.3120289000265299E-2</v>
+      </c>
       <c r="L18" s="22">
-        <v>5.62288806246054E-10</v>
+        <v>2.6809621636045101E-2</v>
       </c>
       <c r="M18" s="23">
-        <v>1.0524092724239948E-9</v>
+        <v>3.3120289000265299E-2</v>
       </c>
       <c r="N18" s="27">
-        <v>1.8716525399999999</v>
+        <v>1.2353881546666667</v>
       </c>
       <c r="O18" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q18" s="22">
-        <v>0.99999999894759073</v>
+        <v>0.96687971099973469</v>
       </c>
       <c r="R18" s="23">
-        <v>0.99999999894759073</v>
+        <v>0.96687971099973469</v>
       </c>
       <c r="S18" s="23">
-        <v>1.6250146500510961E-8</v>
+        <v>0.77479806528170336</v>
       </c>
       <c r="T18" s="23">
-        <v>1.6250146500510961E-8</v>
+        <v>0.77479806528170336</v>
       </c>
       <c r="U18" s="24">
-        <v>3.3333333333333335E-7</v>
+        <v>1</v>
       </c>
       <c r="V18" s="24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="W18" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X18" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y18" s="23">
-        <f t="shared" si="0"/>
-        <v>1.0524092708408261E-9</v>
+        <f t="shared" ref="Y18:Z36" si="0">1-Q18</f>
+        <v>3.3120289000265313E-2</v>
       </c>
       <c r="Z18" s="6">
         <f t="shared" si="0"/>
-        <v>1.0524092708408261E-9</v>
+        <v>3.3120289000265313E-2</v>
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="24">
+        <v>0.342187662</v>
+      </c>
+      <c r="D19" s="24">
         <v>0.995927067</v>
-      </c>
-      <c r="D19" s="24">
-        <v>1.545093896</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>4</v>
@@ -1320,10 +1259,10 @@
         <v>30</v>
       </c>
       <c r="G19" s="23">
-        <v>2.2386621095229898E-6</v>
+        <v>5.62288806246054E-10</v>
       </c>
       <c r="H19" s="6">
-        <v>3.8778607387085781E-6</v>
+        <v>1.0524092724239948E-9</v>
       </c>
       <c r="I19" s="25" t="s">
         <v>31</v>
@@ -1331,59 +1270,59 @@
       <c r="J19" s="23"/>
       <c r="K19" s="6"/>
       <c r="L19" s="22">
-        <v>2.2386621095229898E-6</v>
+        <v>5.62288806246054E-10</v>
       </c>
       <c r="M19" s="23">
-        <v>3.8778607387085781E-6</v>
+        <v>1.0524092724239948E-9</v>
       </c>
       <c r="N19" s="27">
-        <v>1.7322224386666667</v>
+        <v>1.8716525399999999</v>
       </c>
       <c r="O19" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q19" s="22">
-        <v>0.99999612213926126</v>
+        <v>0.99999999894759073</v>
       </c>
       <c r="R19" s="23">
-        <v>0.99999612213926126</v>
+        <v>0.99999999894759073</v>
       </c>
       <c r="S19" s="23">
-        <v>6.46973349652144E-5</v>
+        <v>1.6250146500510961E-8</v>
       </c>
       <c r="T19" s="23">
-        <v>6.46973349652144E-5</v>
+        <v>1.6250146500510961E-8</v>
       </c>
       <c r="U19" s="24">
-        <v>3.3333333333333335E-5</v>
+        <v>3.3333333333333335E-7</v>
       </c>
       <c r="V19" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X19" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y19" s="23">
         <f t="shared" si="0"/>
-        <v>3.8778607387435216E-6</v>
+        <v>1.0524092708408261E-9</v>
       </c>
       <c r="Z19" s="6">
         <f t="shared" si="0"/>
-        <v>3.8778607387435216E-6</v>
+        <v>1.0524092708408261E-9</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="24">
+        <v>0.995927067</v>
+      </c>
+      <c r="D20" s="24">
         <v>1.545093896</v>
-      </c>
-      <c r="D20" s="24">
-        <v>2.5196520410000001</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>4</v>
@@ -1392,10 +1331,10 @@
         <v>30</v>
       </c>
       <c r="G20" s="23">
-        <v>4.4997884737317503E-5</v>
+        <v>2.2386621095229898E-6</v>
       </c>
       <c r="H20" s="6">
-        <v>1.0346862484201612E-4</v>
+        <v>3.8778607387085781E-6</v>
       </c>
       <c r="I20" s="25" t="s">
         <v>31</v>
@@ -1403,59 +1342,59 @@
       <c r="J20" s="23"/>
       <c r="K20" s="6"/>
       <c r="L20" s="22">
-        <v>4.4997884737317503E-5</v>
+        <v>2.2386621095229898E-6</v>
       </c>
       <c r="M20" s="23">
-        <v>1.0346862484201612E-4</v>
+        <v>3.8778607387085781E-6</v>
       </c>
       <c r="N20" s="27">
-        <v>2.2994108600000001</v>
+        <v>1.7322224386666667</v>
       </c>
       <c r="O20" s="28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="22">
-        <v>0.99989653137515799</v>
+        <v>0.99999612213926126</v>
       </c>
       <c r="R20" s="23">
-        <v>0.99989653137515799</v>
+        <v>0.99999612213926126</v>
       </c>
       <c r="S20" s="23">
-        <v>1.3004388689084757E-3</v>
+        <v>6.46973349652144E-5</v>
       </c>
       <c r="T20" s="23">
-        <v>1.3004388689084757E-3</v>
+        <v>6.46973349652144E-5</v>
       </c>
       <c r="U20" s="24">
-        <v>3.3333333333333332E-4</v>
+        <v>3.3333333333333335E-5</v>
       </c>
       <c r="V20" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="X20" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y20" s="23">
         <f t="shared" si="0"/>
-        <v>1.0346862484200692E-4</v>
+        <v>3.8778607387435216E-6</v>
       </c>
       <c r="Z20" s="6">
         <f t="shared" si="0"/>
-        <v>1.0346862484200692E-4</v>
+        <v>3.8778607387435216E-6</v>
       </c>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="24">
+        <v>1.545093896</v>
+      </c>
+      <c r="D21" s="24">
         <v>2.5196520410000001</v>
-      </c>
-      <c r="D21" s="24">
-        <v>3.327915993</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>4</v>
@@ -1464,10 +1403,10 @@
         <v>30</v>
       </c>
       <c r="G21" s="23">
-        <v>2.72088166428101E-6</v>
+        <v>4.4997884737317503E-5</v>
       </c>
       <c r="H21" s="6">
-        <v>5.6531357534758179E-6</v>
+        <v>1.0346862484201612E-4</v>
       </c>
       <c r="I21" s="25" t="s">
         <v>31</v>
@@ -1475,59 +1414,59 @@
       <c r="J21" s="23"/>
       <c r="K21" s="6"/>
       <c r="L21" s="22">
-        <v>2.72088166428101E-6</v>
+        <v>4.4997884737317503E-5</v>
       </c>
       <c r="M21" s="23">
-        <v>5.6531357534758179E-6</v>
+        <v>1.0346862484201612E-4</v>
       </c>
       <c r="N21" s="27">
-        <v>2.0776852693333332</v>
+        <v>2.2994108600000001</v>
       </c>
       <c r="O21" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q21" s="22">
-        <v>0.99999434686424649</v>
+        <v>0.99989653137515799</v>
       </c>
       <c r="R21" s="23">
-        <v>0.99999434686424649</v>
+        <v>0.99989653137515799</v>
       </c>
       <c r="S21" s="23">
-        <v>7.8633480097721185E-5</v>
+        <v>1.3004388689084757E-3</v>
       </c>
       <c r="T21" s="23">
-        <v>7.8633480097721185E-5</v>
+        <v>1.3004388689084757E-3</v>
       </c>
       <c r="U21" s="24">
-        <v>3.3333333333333335E-5</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="V21" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W21" s="24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="X21" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y21" s="23">
         <f t="shared" si="0"/>
-        <v>5.6531357535138937E-6</v>
+        <v>1.0346862484200692E-4</v>
       </c>
       <c r="Z21" s="6">
         <f t="shared" si="0"/>
-        <v>5.6531357535138937E-6</v>
+        <v>1.0346862484200692E-4</v>
       </c>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="24">
+        <v>2.5196520410000001</v>
+      </c>
+      <c r="D22" s="24">
         <v>3.327915993</v>
-      </c>
-      <c r="D22" s="24">
-        <v>4.3705976250000003</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>4</v>
@@ -1536,10 +1475,10 @@
         <v>30</v>
       </c>
       <c r="G22" s="23">
-        <v>4.5974433001425799E-4</v>
+        <v>2.72088166428101E-6</v>
       </c>
       <c r="H22" s="6">
-        <v>1.0989002877769421E-3</v>
+        <v>5.6531357534758179E-6</v>
       </c>
       <c r="I22" s="25" t="s">
         <v>31</v>
@@ -1547,59 +1486,59 @@
       <c r="J22" s="23"/>
       <c r="K22" s="6"/>
       <c r="L22" s="22">
-        <v>4.5974433001425799E-4</v>
+        <v>2.72088166428101E-6</v>
       </c>
       <c r="M22" s="23">
-        <v>1.0989002877769421E-3</v>
+        <v>5.6531357534758179E-6</v>
       </c>
       <c r="N22" s="27">
-        <v>2.3902421760000001</v>
+        <v>2.0776852693333332</v>
       </c>
       <c r="O22" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q22" s="22">
-        <v>0.99890109971222307</v>
+        <v>0.99999434686424649</v>
       </c>
       <c r="R22" s="23">
-        <v>0.99890109971222307</v>
+        <v>0.99999434686424649</v>
       </c>
       <c r="S22" s="23">
-        <v>1.3286611137412056E-2</v>
+        <v>7.8633480097721185E-5</v>
       </c>
       <c r="T22" s="23">
-        <v>1.3286611137412056E-2</v>
+        <v>7.8633480097721185E-5</v>
       </c>
       <c r="U22" s="24">
-        <v>0.01</v>
+        <v>3.3333333333333335E-5</v>
       </c>
       <c r="V22" s="24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W22" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X22" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y22" s="23">
         <f t="shared" si="0"/>
-        <v>1.0989002877769272E-3</v>
+        <v>5.6531357535138937E-6</v>
       </c>
       <c r="Z22" s="6">
         <f t="shared" si="0"/>
-        <v>1.0989002877769272E-3</v>
+        <v>5.6531357535138937E-6</v>
       </c>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="24">
+        <v>3.327915993</v>
+      </c>
+      <c r="D23" s="24">
         <v>4.3705976250000003</v>
-      </c>
-      <c r="D23" s="24">
-        <v>5.6951114260000004</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>4</v>
@@ -1608,10 +1547,10 @@
         <v>30</v>
       </c>
       <c r="G23" s="23">
-        <v>1.26333937706196E-3</v>
+        <v>4.5974433001425799E-4</v>
       </c>
       <c r="H23" s="6">
-        <v>3.494419964082372E-3</v>
+        <v>1.0989002877769421E-3</v>
       </c>
       <c r="I23" s="25" t="s">
         <v>31</v>
@@ -1619,28 +1558,28 @@
       <c r="J23" s="23"/>
       <c r="K23" s="6"/>
       <c r="L23" s="22">
-        <v>1.26333937706196E-3</v>
+        <v>4.5974433001425799E-4</v>
       </c>
       <c r="M23" s="23">
-        <v>3.494419964082372E-3</v>
+        <v>1.0989002877769421E-3</v>
       </c>
       <c r="N23" s="27">
-        <v>2.7660184013333335</v>
+        <v>2.3902421760000001</v>
       </c>
       <c r="O23" s="28" t="s">
         <v>56</v>
       </c>
       <c r="Q23" s="22">
-        <v>0.9965055800359176</v>
+        <v>0.99890109971222307</v>
       </c>
       <c r="R23" s="23">
-        <v>0.9965055800359176</v>
+        <v>0.99890109971222307</v>
       </c>
       <c r="S23" s="23">
-        <v>3.6510507997090644E-2</v>
+        <v>1.3286611137412056E-2</v>
       </c>
       <c r="T23" s="23">
-        <v>3.6510507997090644E-2</v>
+        <v>1.3286611137412056E-2</v>
       </c>
       <c r="U23" s="24">
         <v>0.01</v>
@@ -1656,22 +1595,22 @@
       </c>
       <c r="Y23" s="23">
         <f t="shared" si="0"/>
-        <v>3.4944199640823959E-3</v>
+        <v>1.0989002877769272E-3</v>
       </c>
       <c r="Z23" s="6">
         <f t="shared" si="0"/>
-        <v>3.4944199640823959E-3</v>
+        <v>1.0989002877769272E-3</v>
       </c>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="24">
+        <v>4.3705976250000003</v>
+      </c>
+      <c r="D24" s="24">
         <v>5.6951114260000004</v>
-      </c>
-      <c r="D24" s="24">
-        <v>8.2464557510000009</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>4</v>
@@ -1680,10 +1619,10 @@
         <v>30</v>
       </c>
       <c r="G24" s="23">
-        <v>1.0026818021020699E-3</v>
+        <v>1.26333937706196E-3</v>
       </c>
       <c r="H24" s="6">
-        <v>4.4135971695339225E-3</v>
+        <v>3.494419964082372E-3</v>
       </c>
       <c r="I24" s="25" t="s">
         <v>31</v>
@@ -1691,28 +1630,28 @@
       <c r="J24" s="23"/>
       <c r="K24" s="6"/>
       <c r="L24" s="22">
-        <v>1.0026818021020699E-3</v>
+        <v>1.26333937706196E-3</v>
       </c>
       <c r="M24" s="23">
-        <v>4.4135971695339225E-3</v>
+        <v>3.494419964082372E-3</v>
       </c>
       <c r="N24" s="27">
-        <v>4.401792433333334</v>
+        <v>2.7660184013333335</v>
       </c>
       <c r="O24" s="28" t="s">
         <v>56</v>
       </c>
       <c r="Q24" s="22">
-        <v>0.99558640283046607</v>
+        <v>0.9965055800359176</v>
       </c>
       <c r="R24" s="23">
-        <v>0.99558640283046607</v>
+        <v>0.9965055800359176</v>
       </c>
       <c r="S24" s="23">
-        <v>2.8977504080749821E-2</v>
+        <v>3.6510507997090644E-2</v>
       </c>
       <c r="T24" s="23">
-        <v>2.8977504080749821E-2</v>
+        <v>3.6510507997090644E-2</v>
       </c>
       <c r="U24" s="24">
         <v>0.01</v>
@@ -1728,22 +1667,22 @@
       </c>
       <c r="Y24" s="23">
         <f t="shared" si="0"/>
-        <v>4.4135971695339338E-3</v>
+        <v>3.4944199640823959E-3</v>
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="0"/>
-        <v>4.4135971695339338E-3</v>
+        <v>3.4944199640823959E-3</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="24">
+        <v>5.6951114260000004</v>
+      </c>
+      <c r="D25" s="24">
         <v>8.2464557510000009</v>
-      </c>
-      <c r="D25" s="24">
-        <v>8.9463643600000005</v>
       </c>
       <c r="E25" s="26" t="s">
         <v>4</v>
@@ -1752,10 +1691,10 @@
         <v>30</v>
       </c>
       <c r="G25" s="23">
-        <v>4.7687183333747701E-4</v>
+        <v>1.0026818021020699E-3</v>
       </c>
       <c r="H25" s="6">
-        <v>9.2189410206082781E-4</v>
+        <v>4.4135971695339225E-3</v>
       </c>
       <c r="I25" s="25" t="s">
         <v>31</v>
@@ -1763,59 +1702,59 @@
       <c r="J25" s="23"/>
       <c r="K25" s="6"/>
       <c r="L25" s="22">
-        <v>4.7687183333747701E-4</v>
+        <v>1.0026818021020699E-3</v>
       </c>
       <c r="M25" s="23">
-        <v>9.2189410206082781E-4</v>
+        <v>4.4135971695339225E-3</v>
       </c>
       <c r="N25" s="27">
-        <v>1.9332114786666659</v>
+        <v>4.401792433333334</v>
       </c>
       <c r="O25" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q25" s="22">
-        <v>0.99907810589793922</v>
+        <v>0.99558640283046607</v>
       </c>
       <c r="R25" s="23">
-        <v>0.99907810589793922</v>
+        <v>0.99558640283046607</v>
       </c>
       <c r="S25" s="23">
-        <v>1.3781595983453085E-2</v>
+        <v>2.8977504080749821E-2</v>
       </c>
       <c r="T25" s="23">
-        <v>1.3781595983453085E-2</v>
+        <v>2.8977504080749821E-2</v>
       </c>
       <c r="U25" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="V25" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W25" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X25" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y25" s="23">
         <f t="shared" si="0"/>
-        <v>9.2189410206078293E-4</v>
+        <v>4.4135971695339338E-3</v>
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="0"/>
-        <v>9.2189410206078293E-4</v>
+        <v>4.4135971695339338E-3</v>
       </c>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="24">
+        <v>8.2464557510000009</v>
+      </c>
+      <c r="D26" s="24">
         <v>8.9463643600000005</v>
-      </c>
-      <c r="D26" s="24">
-        <v>9.2968308060000009</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>4</v>
@@ -1824,10 +1763,10 @@
         <v>30</v>
       </c>
       <c r="G26" s="23">
-        <v>5.6920886379173901E-7</v>
+        <v>4.7687183333747701E-4</v>
       </c>
       <c r="H26" s="6">
-        <v>8.3519367382479112E-7</v>
+        <v>9.2189410206082781E-4</v>
       </c>
       <c r="I26" s="25" t="s">
         <v>31</v>
@@ -1835,59 +1774,59 @@
       <c r="J26" s="23"/>
       <c r="K26" s="6"/>
       <c r="L26" s="22">
-        <v>5.6920886379173901E-7</v>
+        <v>4.7687183333747701E-4</v>
       </c>
       <c r="M26" s="23">
-        <v>8.3519367382479112E-7</v>
+        <v>9.2189410206082781E-4</v>
       </c>
       <c r="N26" s="27">
-        <v>1.4672885946666672</v>
+        <v>1.9332114786666659</v>
       </c>
       <c r="O26" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q26" s="22">
-        <v>0.99999916480632622</v>
+        <v>0.99907810589793922</v>
       </c>
       <c r="R26" s="23">
-        <v>0.99999916480632622</v>
+        <v>0.99907810589793922</v>
       </c>
       <c r="S26" s="23">
-        <v>1.6450136163581258E-5</v>
+        <v>1.3781595983453085E-2</v>
       </c>
       <c r="T26" s="23">
-        <v>1.6450136163581258E-5</v>
+        <v>1.3781595983453085E-2</v>
       </c>
       <c r="U26" s="24">
-        <v>3.3333333333333333E-6</v>
+        <v>1E-3</v>
       </c>
       <c r="V26" s="24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W26" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X26" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y26" s="23">
         <f t="shared" si="0"/>
-        <v>8.3519367377604681E-7</v>
+        <v>9.2189410206078293E-4</v>
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="0"/>
-        <v>8.3519367377604681E-7</v>
+        <v>9.2189410206078293E-4</v>
       </c>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="24">
+        <v>8.9463643600000005</v>
+      </c>
+      <c r="D27" s="24">
         <v>9.2968308060000009</v>
-      </c>
-      <c r="D27" s="24">
-        <v>9.7975727730000006</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>4</v>
@@ -1896,10 +1835,10 @@
         <v>30</v>
       </c>
       <c r="G27" s="23">
-        <v>3.2784804284156797E-17</v>
+        <v>5.6920886379173901E-7</v>
       </c>
       <c r="H27" s="6">
-        <v>5.4673774130768381E-17</v>
+        <v>8.3519367382479112E-7</v>
       </c>
       <c r="I27" s="25" t="s">
         <v>31</v>
@@ -1907,59 +1846,59 @@
       <c r="J27" s="23"/>
       <c r="K27" s="6"/>
       <c r="L27" s="22">
-        <v>3.2784804284156797E-17</v>
+        <v>5.6920886379173901E-7</v>
       </c>
       <c r="M27" s="23">
-        <v>5.4673774130768381E-17</v>
+        <v>8.3519367382479112E-7</v>
       </c>
       <c r="N27" s="27">
-        <v>1.6676559559999995</v>
+        <v>1.4672885946666672</v>
       </c>
       <c r="O27" s="28" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q27" s="22">
-        <v>1</v>
+        <v>0.99999916480632622</v>
       </c>
       <c r="R27" s="23">
-        <v>1</v>
+        <v>0.99999916480632622</v>
       </c>
       <c r="S27" s="23">
-        <v>9.4748084381213148E-16</v>
+        <v>1.6450136163581258E-5</v>
       </c>
       <c r="T27" s="23">
-        <v>9.4748084381213148E-16</v>
+        <v>1.6450136163581258E-5</v>
       </c>
       <c r="U27" s="24">
-        <v>3.3333333333333335E-7</v>
+        <v>3.3333333333333333E-6</v>
       </c>
       <c r="V27" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W27" s="24" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="X27" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y27" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3519367377604681E-7</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3519367377604681E-7</v>
       </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="24">
+        <v>9.2968308060000009</v>
+      </c>
+      <c r="D28" s="24">
         <v>9.7975727730000006</v>
-      </c>
-      <c r="D28" s="24">
-        <v>13.197809816000001</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>4</v>
@@ -1968,10 +1907,10 @@
         <v>30</v>
       </c>
       <c r="G28" s="23">
-        <v>6.1195786869129196E-4</v>
+        <v>3.2784804284156797E-17</v>
       </c>
       <c r="H28" s="6">
-        <v>3.3863602871972401E-3</v>
+        <v>5.4673774130768381E-17</v>
       </c>
       <c r="I28" s="25" t="s">
         <v>31</v>
@@ -1979,59 +1918,59 @@
       <c r="J28" s="23"/>
       <c r="K28" s="6"/>
       <c r="L28" s="22">
-        <v>6.1195786869129196E-4</v>
+        <v>3.2784804284156797E-17</v>
       </c>
       <c r="M28" s="23">
-        <v>3.3863602871972401E-3</v>
+        <v>5.4673774130768381E-17</v>
       </c>
       <c r="N28" s="27">
-        <v>5.5336493906666675</v>
+        <v>1.6676559559999995</v>
       </c>
       <c r="O28" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q28" s="22">
-        <v>0.99661363971280281</v>
+        <v>1</v>
       </c>
       <c r="R28" s="23">
-        <v>0.99661363971280281</v>
+        <v>1</v>
       </c>
       <c r="S28" s="23">
-        <v>1.7685582405178337E-2</v>
+        <v>9.4748084381213148E-16</v>
       </c>
       <c r="T28" s="23">
-        <v>1.7685582405178337E-2</v>
+        <v>9.4748084381213148E-16</v>
       </c>
       <c r="U28" s="24">
-        <v>0.01</v>
+        <v>3.3333333333333335E-7</v>
       </c>
       <c r="V28" s="24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W28" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X28" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y28" s="23">
         <f t="shared" si="0"/>
-        <v>3.3863602871971876E-3</v>
+        <v>0</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="0"/>
-        <v>3.3863602871971876E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="24">
+        <v>9.7975727730000006</v>
+      </c>
+      <c r="D29" s="24">
         <v>13.197809816000001</v>
-      </c>
-      <c r="D29" s="24">
-        <v>14.104461709000001</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>4</v>
@@ -2040,10 +1979,10 @@
         <v>30</v>
       </c>
       <c r="G29" s="23">
-        <v>1.4156972664417999E-4</v>
+        <v>6.1195786869129196E-4</v>
       </c>
       <c r="H29" s="6">
-        <v>3.1270900751543092E-4</v>
+        <v>3.3863602871972401E-3</v>
       </c>
       <c r="I29" s="25" t="s">
         <v>31</v>
@@ -2051,59 +1990,59 @@
       <c r="J29" s="23"/>
       <c r="K29" s="6"/>
       <c r="L29" s="22">
-        <v>1.4156972664417999E-4</v>
+        <v>6.1195786869129196E-4</v>
       </c>
       <c r="M29" s="23">
-        <v>3.1270900751543092E-4</v>
+        <v>3.3863602871972401E-3</v>
       </c>
       <c r="N29" s="27">
-        <v>2.2088691906666655</v>
+        <v>5.5336493906666675</v>
       </c>
       <c r="O29" s="28" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q29" s="22">
-        <v>0.99968729099248455</v>
+        <v>0.99661363971280281</v>
       </c>
       <c r="R29" s="23">
-        <v>0.99968729099248455</v>
+        <v>0.99661363971280281</v>
       </c>
       <c r="S29" s="23">
-        <v>4.0913651000168017E-3</v>
+        <v>1.7685582405178337E-2</v>
       </c>
       <c r="T29" s="23">
-        <v>4.0913651000168017E-3</v>
+        <v>1.7685582405178337E-2</v>
       </c>
       <c r="U29" s="24">
-        <v>3.3333333333333332E-4</v>
+        <v>0.01</v>
       </c>
       <c r="V29" s="24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="W29" s="24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="X29" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y29" s="23">
         <f t="shared" si="0"/>
-        <v>3.1270900751545483E-4</v>
+        <v>3.3863602871971876E-3</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="0"/>
-        <v>3.1270900751545483E-4</v>
+        <v>3.3863602871971876E-3</v>
       </c>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="24">
+        <v>13.197809816000001</v>
+      </c>
+      <c r="D30" s="24">
         <v>14.104461709000001</v>
-      </c>
-      <c r="D30" s="24">
-        <v>16.656083170000002</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>4</v>
@@ -2112,10 +2051,10 @@
         <v>30</v>
       </c>
       <c r="G30" s="23">
-        <v>2.33148490314728E-4</v>
+        <v>1.4156972664417999E-4</v>
       </c>
       <c r="H30" s="6">
-        <v>1.0263574122971427E-3</v>
+        <v>3.1270900751543092E-4</v>
       </c>
       <c r="I30" s="25" t="s">
         <v>31</v>
@@ -2123,59 +2062,59 @@
       <c r="J30" s="23"/>
       <c r="K30" s="6"/>
       <c r="L30" s="22">
-        <v>2.33148490314728E-4</v>
+        <v>1.4156972664417999E-4</v>
       </c>
       <c r="M30" s="23">
-        <v>1.0263574122971427E-3</v>
+        <v>3.1270900751543092E-4</v>
       </c>
       <c r="N30" s="27">
-        <v>4.4021619480000025</v>
+        <v>2.2088691906666655</v>
       </c>
       <c r="O30" s="28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q30" s="22">
-        <v>0.99897364258770283</v>
+        <v>0.99968729099248455</v>
       </c>
       <c r="R30" s="23">
-        <v>0.99897364258770283</v>
+        <v>0.99968729099248455</v>
       </c>
       <c r="S30" s="23">
-        <v>6.7379913700956386E-3</v>
+        <v>4.0913651000168017E-3</v>
       </c>
       <c r="T30" s="23">
-        <v>6.7379913700956386E-3</v>
+        <v>4.0913651000168017E-3</v>
       </c>
       <c r="U30" s="24">
-        <v>0.01</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="V30" s="24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W30" s="24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="X30" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y30" s="23">
         <f t="shared" si="0"/>
-        <v>1.0263574122971741E-3</v>
+        <v>3.1270900751545483E-4</v>
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="0"/>
-        <v>1.0263574122971741E-3</v>
+        <v>3.1270900751545483E-4</v>
       </c>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="24">
+        <v>14.104461709000001</v>
+      </c>
+      <c r="D31" s="24">
         <v>16.656083170000002</v>
-      </c>
-      <c r="D31" s="24">
-        <v>17.155520158000002</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>4</v>
@@ -2184,10 +2123,10 @@
         <v>30</v>
       </c>
       <c r="G31" s="23">
-        <v>6.3744180696272295E-5</v>
+        <v>2.33148490314728E-4</v>
       </c>
       <c r="H31" s="6">
-        <v>1.0619244950890422E-4</v>
+        <v>1.0263574122971427E-3</v>
       </c>
       <c r="I31" s="25" t="s">
         <v>31</v>
@@ -2195,59 +2134,59 @@
       <c r="J31" s="23"/>
       <c r="K31" s="6"/>
       <c r="L31" s="22">
-        <v>6.3744180696272295E-5</v>
+        <v>2.33148490314728E-4</v>
       </c>
       <c r="M31" s="23">
-        <v>1.0619244950890422E-4</v>
+        <v>1.0263574122971427E-3</v>
       </c>
       <c r="N31" s="27">
-        <v>1.6659159839999993</v>
+        <v>4.4021619480000025</v>
       </c>
       <c r="O31" s="28" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q31" s="22">
-        <v>0.99989380755049106</v>
+        <v>0.99897364258770283</v>
       </c>
       <c r="R31" s="23">
-        <v>0.99989380755049106</v>
+        <v>0.99897364258770283</v>
       </c>
       <c r="S31" s="23">
-        <v>1.8422068221222692E-3</v>
+        <v>6.7379913700956386E-3</v>
       </c>
       <c r="T31" s="23">
-        <v>1.8422068221222692E-3</v>
+        <v>6.7379913700956386E-3</v>
       </c>
       <c r="U31" s="24">
-        <v>3.3333333333333332E-4</v>
+        <v>0.01</v>
       </c>
       <c r="V31" s="24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="W31" s="24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="X31" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y31" s="23">
         <f t="shared" si="0"/>
-        <v>1.0619244950893503E-4</v>
+        <v>1.0263574122971741E-3</v>
       </c>
       <c r="Z31" s="6">
         <f t="shared" si="0"/>
-        <v>1.0619244950893503E-4</v>
+        <v>1.0263574122971741E-3</v>
       </c>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="24">
+        <v>16.656083170000002</v>
+      </c>
+      <c r="D32" s="24">
         <v>17.155520158000002</v>
-      </c>
-      <c r="D32" s="24">
-        <v>17.802979463</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>4</v>
@@ -2256,10 +2195,10 @@
         <v>30</v>
       </c>
       <c r="G32" s="23">
-        <v>4.7243242271195599E-5</v>
+        <v>6.3744180696272295E-5</v>
       </c>
       <c r="H32" s="6">
-        <v>8.8027344680335383E-5</v>
+        <v>1.0619244950890422E-4</v>
       </c>
       <c r="I32" s="25" t="s">
         <v>31</v>
@@ -2267,28 +2206,28 @@
       <c r="J32" s="23"/>
       <c r="K32" s="6"/>
       <c r="L32" s="22">
-        <v>4.7243242271195599E-5</v>
+        <v>6.3744180696272295E-5</v>
       </c>
       <c r="M32" s="23">
-        <v>8.8027344680335383E-5</v>
+        <v>1.0619244950890422E-4</v>
       </c>
       <c r="N32" s="27">
-        <v>1.8632790733333309</v>
+        <v>1.6659159839999993</v>
       </c>
       <c r="O32" s="28" t="s">
         <v>52</v>
       </c>
       <c r="Q32" s="22">
-        <v>0.99991197265531961</v>
+        <v>0.99989380755049106</v>
       </c>
       <c r="R32" s="23">
-        <v>0.99991197265531961</v>
+        <v>0.99989380755049106</v>
       </c>
       <c r="S32" s="23">
-        <v>1.3653297016375527E-3</v>
+        <v>1.8422068221222692E-3</v>
       </c>
       <c r="T32" s="23">
-        <v>1.3653297016375527E-3</v>
+        <v>1.8422068221222692E-3</v>
       </c>
       <c r="U32" s="24">
         <v>3.3333333333333332E-4</v>
@@ -2304,22 +2243,22 @@
       </c>
       <c r="Y32" s="23">
         <f t="shared" si="0"/>
-        <v>8.8027344680385866E-5</v>
+        <v>1.0619244950893503E-4</v>
       </c>
       <c r="Z32" s="6">
         <f t="shared" si="0"/>
-        <v>8.8027344680385866E-5</v>
+        <v>1.0619244950893503E-4</v>
       </c>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="24">
+        <v>17.155520158000002</v>
+      </c>
+      <c r="D33" s="24">
         <v>17.802979463</v>
-      </c>
-      <c r="D33" s="24">
-        <v>18.605671771000001</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>4</v>
@@ -2328,10 +2267,10 @@
         <v>30</v>
       </c>
       <c r="G33" s="23">
-        <v>6.5227297530628097E-3</v>
+        <v>4.7243242271195599E-5</v>
       </c>
       <c r="H33" s="6">
-        <v>1.3503723086324497E-2</v>
+        <v>8.8027344680335383E-5</v>
       </c>
       <c r="I33" s="25" t="s">
         <v>31</v>
@@ -2339,59 +2278,59 @@
       <c r="J33" s="23"/>
       <c r="K33" s="6"/>
       <c r="L33" s="22">
-        <v>6.5227297530628097E-3</v>
+        <v>4.7243242271195599E-5</v>
       </c>
       <c r="M33" s="23">
-        <v>1.3503723086324497E-2</v>
+        <v>8.8027344680335383E-5</v>
       </c>
       <c r="N33" s="27">
-        <v>2.0702564106666683</v>
+        <v>1.8632790733333309</v>
       </c>
       <c r="O33" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q33" s="22">
-        <v>0.98649627691367547</v>
+        <v>0.99991197265531961</v>
       </c>
       <c r="R33" s="23">
-        <v>0.98649627691367547</v>
+        <v>0.99991197265531961</v>
       </c>
       <c r="S33" s="23">
-        <v>0.18850688986351519</v>
+        <v>1.3653297016375527E-3</v>
       </c>
       <c r="T33" s="23">
-        <v>0.18850688986351519</v>
+        <v>1.3653297016375527E-3</v>
       </c>
       <c r="U33" s="24">
-        <v>1</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="V33" s="24">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="W33" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X33" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y33" s="23">
         <f t="shared" si="0"/>
-        <v>1.3503723086324526E-2</v>
+        <v>8.8027344680385866E-5</v>
       </c>
       <c r="Z33" s="6">
         <f t="shared" si="0"/>
-        <v>1.3503723086324526E-2</v>
+        <v>8.8027344680385866E-5</v>
       </c>
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="24">
+        <v>17.802979463</v>
+      </c>
+      <c r="D34" s="24">
         <v>18.605671771000001</v>
-      </c>
-      <c r="D34" s="24">
-        <v>19.574514854</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>4</v>
@@ -2400,10 +2339,10 @@
         <v>30</v>
       </c>
       <c r="G34" s="23">
-        <v>5.4880372417329002E-8</v>
+        <v>6.5227297530628097E-3</v>
       </c>
       <c r="H34" s="6">
-        <v>1.2577433136265322E-7</v>
+        <v>1.3503723086324497E-2</v>
       </c>
       <c r="I34" s="25" t="s">
         <v>31</v>
@@ -2411,140 +2350,212 @@
       <c r="J34" s="23"/>
       <c r="K34" s="6"/>
       <c r="L34" s="22">
-        <v>5.4880372417329002E-8</v>
+        <v>6.5227297530628097E-3</v>
       </c>
       <c r="M34" s="23">
-        <v>1.2577433136265322E-7</v>
+        <v>1.3503723086324497E-2</v>
       </c>
       <c r="N34" s="27">
-        <v>2.2917907773333326</v>
+        <v>2.0702564106666683</v>
       </c>
       <c r="O34" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q34" s="22">
-        <v>0.99999987422566861</v>
+        <v>0.98649627691367547</v>
       </c>
       <c r="R34" s="23">
-        <v>0.99999987422566861</v>
+        <v>0.98649627691367547</v>
       </c>
       <c r="S34" s="23">
-        <v>1.5860427628608081E-6</v>
+        <v>0.18850688986351519</v>
       </c>
       <c r="T34" s="23">
-        <v>1.5860427628608081E-6</v>
+        <v>0.18850688986351519</v>
       </c>
       <c r="U34" s="24">
-        <v>3.3333333333333335E-7</v>
+        <v>1</v>
       </c>
       <c r="V34" s="24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="W34" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X34" s="24" t="b">
         <v>0</v>
       </c>
       <c r="Y34" s="23">
         <f t="shared" si="0"/>
+        <v>1.3503723086324526E-2</v>
+      </c>
+      <c r="Z34" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3503723086324526E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B35" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="24">
+        <v>18.605671771000001</v>
+      </c>
+      <c r="D35" s="24">
+        <v>19.574514854</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="23">
+        <v>5.4880372417329002E-8</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1.2577433136265322E-7</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J35" s="23"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="22">
+        <v>5.4880372417329002E-8</v>
+      </c>
+      <c r="M35" s="23">
+        <v>1.2577433136265322E-7</v>
+      </c>
+      <c r="N35" s="27">
+        <v>2.2917907773333326</v>
+      </c>
+      <c r="O35" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q35" s="22">
+        <v>0.99999987422566861</v>
+      </c>
+      <c r="R35" s="23">
+        <v>0.99999987422566861</v>
+      </c>
+      <c r="S35" s="23">
+        <v>1.5860427628608081E-6</v>
+      </c>
+      <c r="T35" s="23">
+        <v>1.5860427628608081E-6</v>
+      </c>
+      <c r="U35" s="24">
+        <v>3.3333333333333335E-7</v>
+      </c>
+      <c r="V35" s="24">
+        <v>1</v>
+      </c>
+      <c r="W35" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="X35" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="23">
+        <f t="shared" si="0"/>
         <v>1.257743313942683E-7</v>
       </c>
-      <c r="Z34" s="6">
+      <c r="Z35" s="6">
         <f t="shared" si="0"/>
         <v>1.257743313942683E-7</v>
       </c>
     </row>
-    <row r="35" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="29" t="s">
+    <row r="36" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C36" s="30">
         <v>19.574514854</v>
       </c>
-      <c r="D35" s="30">
+      <c r="D36" s="30">
         <v>20.93</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E36" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="29" t="s">
+      <c r="F36" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G36" s="32">
         <v>3.9992397582768299E-9</v>
       </c>
-      <c r="H35" s="33">
+      <c r="H36" s="33">
         <v>1.1227119875125991E-8</v>
       </c>
-      <c r="I35" s="29" t="s">
+      <c r="I36" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="J35" s="32"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="34">
+      <c r="J36" s="32"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="34">
         <v>3.9992397582768299E-9</v>
       </c>
-      <c r="M35" s="32">
+      <c r="M36" s="32">
         <v>1.1227119875125991E-8</v>
       </c>
-      <c r="N35" s="35">
+      <c r="N36" s="35">
         <v>2.807313527999999</v>
       </c>
-      <c r="O35" s="36" t="s">
+      <c r="O36" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="Q35" s="34">
+      <c r="Q36" s="34">
         <v>0.9999999887728801</v>
       </c>
-      <c r="R35" s="32">
+      <c r="R36" s="32">
         <v>0.9999999887728801</v>
       </c>
-      <c r="S35" s="32">
+      <c r="S36" s="32">
         <v>1.1557802901420038E-7</v>
       </c>
-      <c r="T35" s="32">
+      <c r="T36" s="32">
         <v>1.1557802901420038E-7</v>
       </c>
-      <c r="U35" s="30">
+      <c r="U36" s="30">
         <v>3.3333333333333335E-7</v>
       </c>
-      <c r="V35" s="30">
+      <c r="V36" s="30">
         <v>1</v>
       </c>
-      <c r="W35" s="30" t="s">
+      <c r="W36" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="X35" s="30" t="b">
+      <c r="X36" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="Y35" s="32">
+      <c r="Y36" s="32">
         <f t="shared" si="0"/>
         <v>1.1227119900425464E-8</v>
       </c>
-      <c r="Z35" s="33">
+      <c r="Z36" s="33">
         <f t="shared" si="0"/>
         <v>1.1227119900425464E-8</v>
       </c>
-    </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="Q36" s="37"/>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="Q37" s="37"/>
     </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Q38" s="37"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G16:H35">
+  <conditionalFormatting sqref="G17:H36">
     <cfRule type="expression" dxfId="10" priority="5">
-      <formula>IF($E16="Nee",TRUE,FALSE)</formula>
+      <formula>IF($E17="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16:K35">
+  <conditionalFormatting sqref="J17:K36">
     <cfRule type="expression" dxfId="9" priority="4">
-      <formula>IF($I16="Nee",TRUE,FALSE)</formula>
+      <formula>IF($I17="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O16:O35">
+  <conditionalFormatting sqref="O17:O36">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
@@ -2562,7 +2573,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="endsWith" priority="6" operator="endsWith" id="{3A7D4C1A-2304-4E56-A52D-25A474E72B22}">
-            <xm:f>RIGHT(O16,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
+            <xm:f>RIGHT(O17,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <xm:f>'\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -2573,7 +2584,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="endsWith" priority="7" operator="endsWith" id="{5C89B6F4-368D-4937-BD15-7F247C2F27C7}">
-            <xm:f>RIGHT(O16,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
+            <xm:f>RIGHT(O17,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <xm:f>'\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -2584,7 +2595,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="endsWith" priority="8" operator="endsWith" id="{257B45CB-1734-41CB-8A15-42C75BD2C586}">
-            <xm:f>RIGHT(O16,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
+            <xm:f>RIGHT(O17,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <xm:f>'\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -2595,7 +2606,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="endsWith" priority="9" operator="endsWith" id="{ECF282B4-AC9F-4EA2-8323-47316743E30C}">
-            <xm:f>RIGHT(O16,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
+            <xm:f>RIGHT(O17,LEN('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!))='\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <xm:f>'\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -2606,7 +2617,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="10" operator="containsText" id="{4E6277BD-0FBA-4260-BBCD-63CBDD263560}">
-            <xm:f>NOT(ISERROR(SEARCH('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!,O16)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!,O17)))</xm:f>
             <xm:f>'\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -2617,7 +2628,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="11" operator="containsText" id="{0D6D6E36-CC6B-4C29-AA46-3E144D1690BF}">
-            <xm:f>NOT(ISERROR(SEARCH('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!,O16)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH('\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!,O17)))</xm:f>
             <xm:f>'\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Normen en duidingsklassen'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -2627,7 +2638,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>O16:O35</xm:sqref>
+          <xm:sqref>O17:O36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2637,7 +2648,7 @@
           <x14:formula1>
             <xm:f>'C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\[Benchmartktest_traject 14-2.xlsx]Informatiepagina'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E36:E51 F16:F35</xm:sqref>
+          <xm:sqref>E37:E52 F17:F36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>